<commit_message>
Added commit number to show how the type inference problem was fixed
</commit_message>
<xml_diff>
--- a/Way Forward Documentation.xlsx
+++ b/Way Forward Documentation.xlsx
@@ -244,9 +244,6 @@
     <t>COMMENTS</t>
   </si>
   <si>
-    <t>SOLUTIONS</t>
-  </si>
-  <si>
     <t>EXPECTED OUTCOMES</t>
   </si>
   <si>
@@ -319,9 +316,6 @@
     <t>Help Wanted, time and analysis required.</t>
   </si>
   <si>
-    <t>Done. With Fingers crossed</t>
-  </si>
-  <si>
     <t>Upgrade Runtime dependency to at least version 1.8 and runnable to version 11 (eventually)</t>
   </si>
   <si>
@@ -365,6 +359,12 @@
   </si>
   <si>
     <t>Help Wanted. Seriously help wanted</t>
+  </si>
+  <si>
+    <t>Done. With Fingers crossed. See commit # 635b605 on main</t>
+  </si>
+  <si>
+    <t>SOLUTIONS (Can be raised as issues)</t>
   </si>
 </sst>
 </file>
@@ -870,7 +870,7 @@
   <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,16 +896,16 @@
         <v>75</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I1" s="1"/>
     </row>
@@ -926,7 +926,7 @@
         <v>7</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="1"/>
@@ -935,7 +935,7 @@
       <c r="B3" s="9"/>
       <c r="C3" s="12"/>
       <c r="D3" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>59</v>
@@ -944,7 +944,7 @@
         <v>8</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="1"/>
@@ -960,10 +960,10 @@
         <v>9</v>
       </c>
       <c r="G4" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>85</v>
       </c>
       <c r="I4" s="1"/>
     </row>
@@ -978,10 +978,10 @@
         <v>10</v>
       </c>
       <c r="G5" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>87</v>
       </c>
       <c r="I5" s="1"/>
     </row>
@@ -994,10 +994,10 @@
         <v>11</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I6" s="1"/>
     </row>
@@ -1010,10 +1010,10 @@
         <v>42</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I7" s="1"/>
     </row>
@@ -1026,10 +1026,10 @@
         <v>14</v>
       </c>
       <c r="G8" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>91</v>
       </c>
       <c r="I8" s="1"/>
     </row>
@@ -1039,13 +1039,13 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I9" s="1"/>
     </row>
@@ -1096,18 +1096,18 @@
         <v>2</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="2:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B14" s="9"/>
       <c r="C14" s="12"/>
       <c r="D14" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>59</v>
@@ -1116,10 +1116,10 @@
         <v>6</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I14" s="1"/>
     </row>
@@ -1127,7 +1127,7 @@
       <c r="B15" s="9"/>
       <c r="C15" s="12"/>
       <c r="D15" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>60</v>
@@ -1136,10 +1136,10 @@
         <v>3</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I15" s="1"/>
     </row>
@@ -1151,13 +1151,13 @@
         <v>61</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I16" s="1"/>
     </row>
@@ -1167,13 +1167,13 @@
       <c r="D17" s="15"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I17" s="1"/>
     </row>
@@ -1186,10 +1186,10 @@
         <v>5</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I18" s="1"/>
     </row>
@@ -1202,10 +1202,10 @@
         <v>36</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I19" s="1"/>
     </row>
@@ -1239,7 +1239,7 @@
       <c r="H22" s="6"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="11" t="s">
         <v>21</v>
@@ -1257,10 +1257,10 @@
         <v>19</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I23" s="1"/>
     </row>
@@ -1278,10 +1278,10 @@
         <v>20</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I24" s="1"/>
     </row>
@@ -1333,10 +1333,10 @@
       <c r="H28" s="7"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>1</v>
@@ -1351,14 +1351,14 @@
         <v>24</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -1370,10 +1370,10 @@
         <v>25</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I30" s="1"/>
     </row>
@@ -1441,10 +1441,10 @@
         <v>15</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H35" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I35" s="1"/>
     </row>
@@ -1460,10 +1460,10 @@
         <v>18</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I36" s="1"/>
     </row>
@@ -1477,10 +1477,10 @@
         <v>16</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I37" s="1"/>
     </row>
@@ -1494,10 +1494,10 @@
         <v>17</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I38" s="1"/>
     </row>
@@ -1552,14 +1552,14 @@
         <v>46</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
@@ -1573,10 +1573,10 @@
         <v>47</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I43" s="1"/>
     </row>
@@ -1589,13 +1589,13 @@
       </c>
       <c r="E44" s="6"/>
       <c r="F44" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I44" s="1"/>
     </row>
@@ -1611,10 +1611,10 @@
         <v>48</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I45" s="1"/>
     </row>
@@ -1628,10 +1628,10 @@
         <v>49</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I46" s="1"/>
     </row>
@@ -1645,10 +1645,10 @@
         <v>50</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I47" s="1"/>
     </row>
@@ -1662,10 +1662,10 @@
         <v>51</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I48" s="1"/>
     </row>
@@ -1679,10 +1679,10 @@
         <v>52</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I49" s="1"/>
     </row>
@@ -1696,10 +1696,10 @@
         <v>53</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I50" s="1"/>
     </row>
@@ -1754,10 +1754,10 @@
         <v>34</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I54" s="1"/>
     </row>
@@ -1775,10 +1775,10 @@
         <v>37</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I55" s="1"/>
     </row>
@@ -1794,10 +1794,10 @@
         <v>38</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I56" s="1"/>
     </row>
@@ -1811,10 +1811,10 @@
         <v>39</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I57" s="1"/>
     </row>
@@ -1828,10 +1828,10 @@
         <v>40</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I58" s="1"/>
     </row>
@@ -1845,10 +1845,10 @@
         <v>41</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I59" s="1"/>
     </row>

</xml_diff>

<commit_message>
[skip-ci] highlighted in the way forward excel the issues which are already raised
</commit_message>
<xml_diff>
--- a/Way Forward Documentation.xlsx
+++ b/Way Forward Documentation.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Way Ahead Dashboard Draft" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" calcOnSave="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -388,12 +388,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -507,7 +513,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -564,6 +570,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -869,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,7 +1050,7 @@
       <c r="C9" s="12"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="20" t="s">
         <v>91</v>
       </c>
       <c r="G9" s="6" t="s">
@@ -1092,7 +1104,7 @@
       <c r="E13" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="21" t="s">
         <v>2</v>
       </c>
       <c r="G13" s="5" t="s">
@@ -1182,7 +1194,7 @@
       <c r="C18" s="12"/>
       <c r="D18" s="15"/>
       <c r="E18" s="6"/>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="20" t="s">
         <v>5</v>
       </c>
       <c r="G18" s="6" t="s">

</xml_diff>